<commit_message>
se agregaron funcionalidades de cartel en crear tarea si no esta completo los campos requeridos
</commit_message>
<xml_diff>
--- a/derivadorDeTareas/pruebas unitarias.xlsx
+++ b/derivadorDeTareas/pruebas unitarias.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\cursos\2024  coder python\python TPS\Preentrega_3_Chiesa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\cursos\2024  coder python\python TPS\Preentrega_3_Chiesa\derivadorDeTareas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{42EF970E-3688-4BEE-BEBF-4DA57ECD309C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA3BE17-CF03-4F16-80AB-7F1B0332E3C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{058FCB3E-7D89-462C-8DFF-C09A8A10797A}"/>
+    <workbookView xWindow="28665" yWindow="-135" windowWidth="20760" windowHeight="11070" xr2:uid="{058FCB3E-7D89-462C-8DFF-C09A8A10797A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="55">
   <si>
     <t>Tabla de Pruebas Unitarias</t>
   </si>
@@ -128,9 +128,6 @@
     <t>Acceso permitido, se muestra el menú de administración</t>
   </si>
   <si>
-    <t>Usuario regular</t>
-  </si>
-  <si>
     <t>Crear Tarea</t>
   </si>
   <si>
@@ -185,21 +182,6 @@
     <t>Lista de tareas del usuario</t>
   </si>
   <si>
-    <t>Detalle de Tarea</t>
-  </si>
-  <si>
-    <t>Ver detalles de una tarea específica</t>
-  </si>
-  <si>
-    <t>ID de tarea</t>
-  </si>
-  <si>
-    <t>Acceder a /tarea/&lt;id&gt;/</t>
-  </si>
-  <si>
-    <t>Detalles de la tarea mostrados</t>
-  </si>
-  <si>
     <t>Comentarios</t>
   </si>
   <si>
@@ -215,73 +197,10 @@
     <t>Comentario añadido y mostrado en los detalles de la tarea</t>
   </si>
   <si>
-    <t>Lista de Usuarios</t>
-  </si>
-  <si>
-    <t>Ver lista de usuarios como administrador</t>
-  </si>
-  <si>
-    <t>Acceder a /usuarios/</t>
-  </si>
-  <si>
-    <t>Lista de usuarios mostrada</t>
-  </si>
-  <si>
-    <t>Editar Usuario</t>
-  </si>
-  <si>
-    <t>Editar información de un usuario</t>
-  </si>
-  <si>
-    <t>Datos actualizados del usuario</t>
-  </si>
-  <si>
-    <t>Enviar formulario de edición de usuario</t>
-  </si>
-  <si>
-    <t>Usuario actualizado correctamente</t>
-  </si>
-  <si>
-    <t>Eliminar Usuario</t>
-  </si>
-  <si>
-    <t>Intentar eliminar usuario como administrador</t>
-  </si>
-  <si>
-    <t>Intentar eliminar usuario</t>
-  </si>
-  <si>
-    <t>Usuario eliminado correctamente</t>
-  </si>
-  <si>
-    <t>Eliminar Tarea</t>
-  </si>
-  <si>
-    <t>Intentar eliminar tarea como administrador</t>
-  </si>
-  <si>
-    <t>Administrador</t>
-  </si>
-  <si>
-    <t>Intentar eliminar tarea</t>
-  </si>
-  <si>
-    <t>Tarea eliminada correctamente</t>
-  </si>
-  <si>
-    <t>Intentar eliminar tarea como usuario</t>
-  </si>
-  <si>
-    <t>Error: Permiso denegado, solo administrador puede eliminar</t>
-  </si>
-  <si>
-    <t>OK</t>
-  </si>
-  <si>
     <t>redireccion a pagina de login</t>
   </si>
   <si>
-    <t>ok</t>
+    <t>Pasa</t>
   </si>
 </sst>
 </file>
@@ -374,7 +293,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>3124200</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>1732722</xdr:rowOff>
+      <xdr:rowOff>1736532</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -416,7 +335,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>2044656</xdr:colOff>
+      <xdr:colOff>2040846</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>1674167</xdr:rowOff>
     </xdr:to>
@@ -460,9 +379,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>2915767</xdr:colOff>
+      <xdr:colOff>2911957</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>1200261</xdr:rowOff>
+      <xdr:rowOff>1196451</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -487,6 +406,446 @@
         <a:xfrm>
           <a:off x="5085431" y="6575282"/>
           <a:ext cx="2524190" cy="1183566"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>13608</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>52523</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1584098</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>819510</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B1ED97E-7551-B9F8-B239-E48D4F66D614}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4721679" y="7876630"/>
+          <a:ext cx="1581920" cy="770797"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1483180</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3794758</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>703762</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagen 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F51B459F-D199-472D-6797-6A68BCF4F6FB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6191251" y="7919357"/>
+          <a:ext cx="2307768" cy="612322"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>13608</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>54429</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1984739</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>951581</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagen 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41152A99-F9AF-1BD9-E053-A5B31AB096EE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4721679" y="8790215"/>
+          <a:ext cx="1971131" cy="897152"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1875880</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>66131</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3602083</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1008382</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Imagen 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED237A77-8D9C-CD4D-C699-953E5EF6BF1C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6583951" y="8801917"/>
+          <a:ext cx="1730013" cy="955586"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>132264</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>235132</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1694481</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>853441</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Imagen 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09FBFE40-16F3-0CB4-722B-F256C211A20E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4840335" y="10073096"/>
+          <a:ext cx="1577457" cy="618309"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1710693</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>75657</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3792312</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>970317</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Imagen 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA2EBD9C-367A-CF6E-4B59-27E3732D5430}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6418764" y="9913621"/>
+          <a:ext cx="2070189" cy="902280"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>270238</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>153487</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1849436</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>892235</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Imagen 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BC02533-B6E7-21DD-D4BC-2AC8FAB7331B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4978309" y="11066416"/>
+          <a:ext cx="1571578" cy="746368"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2076179</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>97425</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3883600</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1275261</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Imagen 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BEC52CB-CAB4-3160-693D-009E5577A16B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6784250" y="11010354"/>
+          <a:ext cx="1807421" cy="1181646"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>122465</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>68036</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1712596</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>164720</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Imagen 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4ACB9452-A9C1-82F1-EF98-675E5D436F02}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5660572" y="12300857"/>
+          <a:ext cx="1590131" cy="1006458"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2180952</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>71847</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3733896</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>68035</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Imagen 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{470EC378-EB93-7F39-8F2F-0B2BF78BCF3D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7719059" y="12304668"/>
+          <a:ext cx="1552944" cy="909772"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -815,20 +1174,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0909F9DE-23E3-4881-8EDA-E17FD08596A2}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.21875" customWidth="1"/>
-    <col min="2" max="2" width="14.21875" customWidth="1"/>
-    <col min="3" max="3" width="10.21875" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" customWidth="1"/>
     <col min="4" max="4" width="12.21875" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" customWidth="1"/>
-    <col min="6" max="6" width="10.21875" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="58.6640625" customWidth="1"/>
     <col min="8" max="8" width="10.21875" customWidth="1"/>
   </cols>
@@ -894,7 +1253,7 @@
         <v>13</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="152.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -918,7 +1277,7 @@
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
@@ -941,10 +1300,10 @@
         <v>21</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>80</v>
+        <v>53</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="145.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -968,7 +1327,7 @@
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="99" customHeight="1" x14ac:dyDescent="0.3">
@@ -992,7 +1351,7 @@
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="72" x14ac:dyDescent="0.3">
@@ -1000,246 +1359,119 @@
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
+      <c r="H9" s="2" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
+      <c r="H10" s="2" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="11" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="84.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
+      <c r="H11" s="2" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="12" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="104.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
+      <c r="H12" s="2" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="13" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
-        <v>11</v>
-      </c>
-      <c r="B14" s="2" t="s">
+      <c r="H13" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="1:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
-        <v>12</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-    </row>
-    <row r="16" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
-        <v>13</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
-        <v>14</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-    </row>
-    <row r="18" spans="1:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
-        <v>15</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-    </row>
-    <row r="19" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
-        <v>16</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>